<commit_message>
Went once-through, now runs top-to-bottom
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Post-Questionnaire_TG.xlsx
+++ b/raw-data-prep/raw_data/Post-Questionnaire_TG.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="55">
   <si>
     <t>Subject</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>6- note- lol</t>
   </si>
   <si>
     <t>3.34 C, 3.4 HS</t>
@@ -570,7 +567,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15"/>
@@ -3833,8 +3830,8 @@
       <c r="B29" s="2">
         <v>1</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>47</v>
+      <c r="C29" s="2">
+        <v>6</v>
       </c>
       <c r="D29" s="2">
         <v>3</v>
@@ -4519,7 +4516,7 @@
         <v>1</v>
       </c>
       <c r="AL34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:38">
@@ -5325,7 +5322,7 @@
         <v>20</v>
       </c>
       <c r="AJ41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AK41">
         <v>3</v>
@@ -5447,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="AL42" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:38">
@@ -8115,7 +8112,7 @@
         <v>1</v>
       </c>
       <c r="AL65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:38">
@@ -8460,7 +8457,7 @@
         <v>5</v>
       </c>
       <c r="AK68" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AL68">
         <v>2.7</v>
@@ -8781,7 +8778,7 @@
         <v>5</v>
       </c>
       <c r="AB71" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC71" s="1"/>
       <c r="AD71" s="1"/>
@@ -10296,7 +10293,7 @@
         <v>5</v>
       </c>
       <c r="AK84" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AL84" s="2">
         <v>2.75</v>
@@ -12565,7 +12562,7 @@
         <v>6</v>
       </c>
       <c r="AB104" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC104" s="1"/>
       <c r="AD104" s="1"/>
@@ -12695,7 +12692,7 @@
         <v>289</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -14833,7 +14830,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>

</xml_diff>